<commit_message>
commit on 2022-10-04 at 17:18:03
</commit_message>
<xml_diff>
--- a/submissions/pending.xlsx
+++ b/submissions/pending.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/distasl/Documents/WD/profDocs/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CF3C4F-0D8E-0E4F-91E4-0F0038E7F071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DA7439-0959-AE4B-9D89-64554F8905EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{9CE22EEB-E98C-5749-B029-6028B6AD91A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="pending" localSheetId="0">Sheet1!$A$1:$E$31</definedName>
+    <definedName name="pending" localSheetId="0">Sheet1!$A$1:$E$35</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{07F63036-0552-B548-9A30-B1EB02866FB1}" name="pending" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/distasl/Documents/WD/profDocs/submissions/pending.txt" tab="0" comma="1">
+    <textPr sourceFile="/Users/distasl/Documents/WD/profDocs/submissions/pending.txt" tab="0" comma="1">
       <textFields count="5">
         <textField type="text"/>
         <textField type="text"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="71">
   <si>
     <t>Institute of Science and Technology Austria (ISTA)</t>
   </si>
@@ -63,9 +63,6 @@
     <t xml:space="preserve"> Assistant Professor (tenure-track) and Professor positions in all areas of sciences</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.nature.com/naturecareers/job/assistant-professor-tenuretrack-and-professor-positions-in-all-areas-of-sciences-institute-of-science-and-technology-austria-ista-762911</t>
-  </si>
-  <si>
     <t>King Fahd University of Petroleum &amp; Minerals</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t xml:space="preserve"> Assistant / Associate / Full Professor - Material Science and Engineering</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://jobs.kfupm.edu.sa/postings/1813</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t xml:space="preserve"> Postdoc in network-inspired models of heterogeneous materials</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.nature.com/naturecareers/job/postdoc-in-networkinspired-models-of-heterogeneous-materials-aarhus-university-au-763330</t>
-  </si>
-  <si>
     <t>Syracuse University</t>
   </si>
   <si>
@@ -102,9 +93,6 @@
     <t xml:space="preserve"> Assistant Professor- Solid Mechanics</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.sujobopps.com/postings/94961</t>
-  </si>
-  <si>
     <t>Ghent University</t>
   </si>
   <si>
@@ -114,9 +102,6 @@
     <t xml:space="preserve"> Postdoc vacancy on computational mechanics of thick adhesive joints in large wind turbine blades</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://composites.ugent.be/PhD_job_vacancies_PhD_job_positions_composites.html</t>
-  </si>
-  <si>
     <t>Technology Innovation Institute</t>
   </si>
   <si>
@@ -126,45 +111,30 @@
     <t xml:space="preserve"> Senior Researcher</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://imechanica.org/node/26244</t>
-  </si>
-  <si>
     <t>University of Southern Denmark</t>
   </si>
   <si>
     <t xml:space="preserve"> Postdoc Position in Soft Robotic Locomotion Control and Learning</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.sdu.dk/en/service/ledige_stillinger/1195449</t>
-  </si>
-  <si>
     <t>Georgia Tech</t>
   </si>
   <si>
     <t xml:space="preserve"> Multi Rank Tenured/Tenure-Track Faculty Positions</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://careers.hprod.onehcm.usg.edu/psc/careers/CAREERS/HRMS/c/HRS_HRAM_FL.HRS_CG_SEARCH_FL.GBL?Page=HRS_APP_SCHJOB_FL&amp;Action=U</t>
-  </si>
-  <si>
     <t>Colorado School of Mines</t>
   </si>
   <si>
     <t xml:space="preserve"> Assistant Professor Mechanical Engineering Biomechanics</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://jobs.mines.edu/cw/en-us/job/495861/assistant-professor-mechanical-engineering-biomechanics</t>
-  </si>
-  <si>
     <t>UC San Diego</t>
   </si>
   <si>
     <t xml:space="preserve"> Assistant Professor in Aerospace Engineering</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://apol-recruit.ucsd.edu/JPF03339</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Assistant Teaching Professor (LPSOE) in Aerospace Engineering</t>
   </si>
   <si>
@@ -174,9 +144,6 @@
     <t xml:space="preserve"> Assistant or Associate Professor of Mechanical Engineering - Biomechanics</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://careers.purdue.edu/job/West-Lafayette-Assistant-or-Associate-Professor-of-Mechanical-Engineering-Biomechanics-IN-47906/932366300/</t>
-  </si>
-  <si>
     <t>University of Exeter</t>
   </si>
   <si>
@@ -186,72 +153,45 @@
     <t xml:space="preserve"> Lectureship with initial Research Fellowship in Materials Modelling and Simulation</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://jobs.exeter.ac.uk/hrpr_webrecruitment/wrd/run/ETREC107GF.open?VACANCY_ID=448681b4fm&amp;WVID=3817591jNg&amp;LANG=USA</t>
-  </si>
-  <si>
     <t>University of Nottingham</t>
   </si>
   <si>
     <t xml:space="preserve"> Nottingham Research Fellowships 2023</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.nottingham.ac.uk/jobs/currentvacancies/ref/NARF2023</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Assistant or Associate Professor in Solid Mechanics</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.sdu.dk/en/service/ledige_stillinger/1196606</t>
-  </si>
-  <si>
-    <t>Pale Blue Dot¬ÆRecruitment Limited</t>
-  </si>
-  <si>
     <t xml:space="preserve"> IE</t>
   </si>
   <si>
     <t xml:space="preserve"> R&amp;D Engineer</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3124936927/?refId=943fb5ac-7d12-48fa-82c9-728b874e7b54&amp;trackingId=ncNGSaq3TFuRcNdtLWYfjA%3D%3D&amp;trk=flagship3_job_home_savedjobs</t>
-  </si>
-  <si>
     <t>Raytheon UK</t>
   </si>
   <si>
     <t xml:space="preserve"> Senior Mechanical Engineer</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3249299200/?refId=943fb5ac-7d12-48fa-82c9-728b874e7b54&amp;trackingId=V14blwBhRleNexF35IjHMg%3D%3D&amp;trk=flagship3_job_home_savedjobs</t>
-  </si>
-  <si>
     <t>Hays</t>
   </si>
   <si>
     <t xml:space="preserve"> Senior Mechanical Design Engineer</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3252949620/?refId=943fb5ac-7d12-48fa-82c9-728b874e7b54&amp;trackingId=iskLuf5pTmiMMUqzNQDOjQ%3D%3D&amp;trk=flagship3_job_home_savedjobs</t>
-  </si>
-  <si>
     <t>Floating Power Plant</t>
   </si>
   <si>
     <t xml:space="preserve"> Research &amp; Development Naval Architect/Structural Engineer</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3146724454/?refId=943fb5ac-7d12-48fa-82c9-728b874e7b54&amp;trackingId=dZtuxDeDTg6v071cpRk0XQ%3D%3D&amp;trk=flagship3_job_home_savedjobs</t>
-  </si>
-  <si>
     <t>ServiceNow</t>
   </si>
   <si>
     <t xml:space="preserve"> EMEA Learning Manager</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3225612167/?alternateChannel=search&amp;refId=lJVuGicyUSnYYZkbYO6qzQ%3D%3D&amp;trackingId=0i56ToJcMXot%2FAJETWTlBQ%3D%3D&amp;trk=d_flagship3_search_srp_jobs</t>
-  </si>
-  <si>
     <t>Wikimedia Foundation</t>
   </si>
   <si>
@@ -261,9 +201,6 @@
     <t xml:space="preserve"> Technical Community Program Manager</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://boards.greenhouse.io/wikimedia/jobs/4496668</t>
-  </si>
-  <si>
     <t>RavenPack</t>
   </si>
   <si>
@@ -273,80 +210,79 @@
     <t xml:space="preserve"> Quantitative Researcher</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3256966142/?alternateChannel=search&amp;refId=dAsMlpfljPkYMRsHnYIdcQ%3D%3D&amp;trackingId=0glUOyL4W8jbKnes5%2BtPpQ%3D%3D</t>
-  </si>
-  <si>
     <t>NKT Photonics</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3263086882/?lgTemp=jobs_jymbii_digest&amp;eBP=NotAvailableFromMidTier&amp;lgCta=eml-jymbii-organic-job-card&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=YLoLkXJTqwcLrXKNgxEN6g%3D%3D&amp;trackingId=YLoLkXJTqwcLrXKNgxEN6g%3D%3D&amp;midToken=AQGW6lN0ZhE6Zw&amp;midSig=0gTDfJlgZaeqs1&amp;trk=eml-jobs_jymbii_digest-jymbii-43-job_card_mercado&amp;trkEmail=eml-jobs_jymbii_digest-jymbii-43-job_card_mercado-null-242drh%7El8ijz7de%7Edh-null-jobs%7Eview</t>
-  </si>
-  <si>
     <t>Mason Alexander</t>
   </si>
   <si>
     <t xml:space="preserve"> R&amp;D Technical Lead</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3278517624/?lgTemp=jobs_jymbii_digest&amp;eBP=NotAvailableFromMidTier&amp;lgCta=eml-jymbii-organic-job-card&amp;recommendedFlavor=HIDDEN_GEM&amp;refId=2CypfbVUooL1DKQxBBqnlg%3D%3D&amp;trackingId=2CypfbVUooL1DKQxBBqnlg%3D%3D&amp;midToken=AQGW6lN0ZhE6Zw&amp;midSig=1qW8sQGH0J7qs1&amp;trk=eml-jobs_jymbii_digest-jymbii-33-job_card_mercado&amp;trkEmail=eml-jobs_jymbii_digest-jymbii-33-job_card_mercado-null-242drh%7El8beweas%7Euf-null-jobs%7Eview</t>
-  </si>
-  <si>
     <t>UNICEF</t>
   </si>
   <si>
     <t xml:space="preserve"> Innovation Manager (WASH)</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3276000844/?lgTemp=jobs_jymbii_digest&amp;eBP=NotAvailableFromMidTier&amp;lgCta=eml-jymbii-organic-job-card&amp;recommendedFlavor=SCHOOL_RECRUIT&amp;refId=yGQcs9ybSngEdWVlEW7v3Q%3D%3D&amp;trackingId=yGQcs9ybSngEdWVlEW7v3Q%3D%3D&amp;midToken=AQGW6lN0ZhE6Zw&amp;midSig=0KvbZl5i5Aaas1&amp;trk=eml-jobs_jymbii_digest-jymbii-27-job_card_mercado&amp;trkEmail=eml-jobs_jymbii_digest-jymbii-27-job_card_mercado-null-242drh%7El8e9fvwr%7Exe-null-jobs%7Eview</t>
-  </si>
-  <si>
     <t>Fiberline Composites</t>
   </si>
   <si>
     <t xml:space="preserve"> Project Manager</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.innomate.com/InnomatePublicPagesMedarb/JobNotice.aspx?CompanyId=fiberline&amp;JobNoticeId=122</t>
-  </si>
-  <si>
     <t>Hollister</t>
   </si>
   <si>
     <t xml:space="preserve"> Senior R&amp;D Engineer</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3264064488/?refId=V%2FHpkFDpy62s7woTWC5YmQ%3D%3D&amp;trackingId=V%2FHpkFDpy62s7woTWC5YmQ%3D%3D&amp;midToken=AQGW6lN0ZhE6Zw&amp;midSig=0FiJf_T0kfjas1&amp;trk=eml-email_jobs_viewed_job_reminder_01-similar_jobs-64-similar%7Ejob%7Etitle%7Emercado&amp;trkEmail=eml-email_jobs_viewed_job_reminder_01-similar_jobs-64-similar%7Ejob%7Etitle%7Emercado-null-242drh%7El8nbn0pw%7E30-null-jobs%7Eview</t>
-  </si>
-  <si>
     <t>Real Staffing</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3270262889/?refId=NXgPyne2BuIGhBW0wEsRbQ%3D%3D&amp;trackingId=NXgPyne2BuIGhBW0wEsRbQ%3D%3D&amp;midToken=AQGW6lN0ZhE6Zw&amp;midSig=0FiJf_T0kfjas1&amp;trk=eml-email_jobs_viewed_job_reminder_01-similar_jobs-60-similar%7Ejob%7Etitle%7Emercado&amp;trkEmail=eml-email_jobs_viewed_job_reminder_01-similar_jobs-60-similar%7Ejob%7Etitle%7Emercado-null-242drh%7El8nbn0pw%7E30-null-jobs%7Eview</t>
-  </si>
-  <si>
     <t>Julia Computing</t>
   </si>
   <si>
     <t xml:space="preserve"> Application Developer</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://jobs.juliacomputing.com/jobs/3NhVYuObq6cY/application-developer-remote</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Scientific Application Developer</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://jobs.juliacomputing.com/jobs/Ievy9W70_BjO/scientific-application-developer-remote</t>
+    <t>Pale Blue DotÂ®Recruitment Limited</t>
+  </si>
+  <si>
+    <t>Novo Nordisk</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Research Data Steward</t>
+  </si>
+  <si>
+    <t>Carpentries</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Executive Council</t>
+  </si>
+  <si>
+    <t>view</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -369,18 +305,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -697,7 +639,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526B7EBF-53BB-884F-AAF1-E7894D9216BC}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
@@ -712,67 +654,67 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>47</v>
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E1" s="2">
-        <v>44840</v>
+        <v>44858</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="2">
-        <v>44848</v>
+        <v>15</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E3" s="2">
-        <v>44848</v>
+        <v>44849</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E4" s="2">
         <v>44849</v>
@@ -780,434 +722,543 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E5" s="2">
-        <v>44849</v>
+        <v>44880</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="2">
-        <v>44849</v>
+        <v>43</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="2">
-        <v>44851</v>
+        <v>39</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="2">
-        <v>44855</v>
+        <v>56</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="2">
-        <v>44858</v>
+        <v>58</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="E10" s="2">
-        <v>44871</v>
+        <v>44857</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>49</v>
+        <v>60</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E11" s="2">
-        <v>44880</v>
+        <v>44865</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>40</v>
+        <v>67</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E12" s="2">
-        <v>44896</v>
+        <v>44843</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
+        <v>51</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
+        <v>37</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
+        <v>60</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>78</v>
+        <v>48</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>81</v>
+        <v>63</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" t="s">
-        <v>8</v>
+        <v>64</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" t="s">
-        <v>8</v>
+        <v>69</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="2">
+        <v>44851</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>53</v>
+        <v>32</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="2">
+        <v>44871</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>62</v>
+        <v>34</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="2">
+        <v>44840</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>73</v>
+        <v>41</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>89</v>
+        <v>12</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="2">
+        <v>44849</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>94</v>
+        <v>22</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="2">
+        <v>44851</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="2">
+        <v>44855</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="2">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="2">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="2">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:E34">
-    <sortCondition ref="E1:E34"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E35">
+    <sortCondition ref="B1:B35"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{4B133E65-D92E-1543-AA75-04310E5BFC1E}"/>
+    <hyperlink ref="D11" r:id="rId2" xr:uid="{20B84960-8C50-A742-979E-A5D4829F3DC1}"/>
+    <hyperlink ref="D12" r:id="rId3" xr:uid="{D64DBDE8-111D-794C-9523-567730D88024}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{99799B85-16A3-A14B-A8E7-450FC0E3092D}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{98BADD85-0200-FC4B-AED6-28EF3DFBAA0A}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{32CD9F87-5983-694F-81E4-624893AC0C09}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{62232260-DB6F-9A40-9A29-0DE8F7884E68}"/>
+    <hyperlink ref="D33" r:id="rId8" xr:uid="{A88AFDAB-EB57-A44F-B93A-4A64DFE6CE6B}"/>
+    <hyperlink ref="D1" r:id="rId9" xr:uid="{5806C2F7-7A0A-1B42-975F-24FC659F7AF3}"/>
+    <hyperlink ref="D2" r:id="rId10" xr:uid="{7FDB8605-1B30-F741-B74B-95E2C37C703E}"/>
+    <hyperlink ref="D3" r:id="rId11" xr:uid="{E46C9387-595E-A146-A5C6-2F52A948F1B8}"/>
+    <hyperlink ref="D4" r:id="rId12" xr:uid="{29ABE021-E5BF-BA48-8FE8-FFBBF41B5B18}"/>
+    <hyperlink ref="D5" r:id="rId13" xr:uid="{7E7C2147-CD4A-914F-9E39-17834782CD24}"/>
+    <hyperlink ref="D13" r:id="rId14" xr:uid="{A1881E4E-16C6-A047-9D87-49FBF3BA885E}"/>
+    <hyperlink ref="D14" r:id="rId15" xr:uid="{58C4C5F6-D88E-6A41-8286-DFE5ABE5AFE4}"/>
+    <hyperlink ref="D15" r:id="rId16" xr:uid="{11361235-E0CA-5742-91A1-FC72BEFBFCD9}"/>
+    <hyperlink ref="D16" r:id="rId17" xr:uid="{1F055798-6460-5E4E-B1EE-F251CB0F6DBE}"/>
+    <hyperlink ref="D17" r:id="rId18" xr:uid="{7C62CE5E-6D3E-174A-B7A6-66AE57580976}"/>
+    <hyperlink ref="D18" r:id="rId19" xr:uid="{A1301579-4623-604F-87B9-862DAC929BAD}"/>
+    <hyperlink ref="D19" r:id="rId20" xr:uid="{3124D040-ACDD-0747-8E1B-5B8DCD5F3F5F}"/>
+    <hyperlink ref="D20" r:id="rId21" xr:uid="{47AF3DA8-DF4A-4D47-96DA-0FF7BA634481}"/>
+    <hyperlink ref="D21" r:id="rId22" xr:uid="{4EC961BF-5212-1547-ABC6-F12C92CDF8DA}"/>
+    <hyperlink ref="D22" r:id="rId23" xr:uid="{7984A528-6DCD-9340-85FB-95BC4BF499E7}"/>
+    <hyperlink ref="D23" r:id="rId24" xr:uid="{67B3F2F8-C645-DF47-B54D-F50486927AB7}"/>
+    <hyperlink ref="D24" r:id="rId25" xr:uid="{857C5379-06A9-614F-9C37-5F7E3B71FC07}"/>
+    <hyperlink ref="D25" r:id="rId26" xr:uid="{D46B45D8-1EEB-E84A-9A6D-8419E5353BC9}"/>
+    <hyperlink ref="D26" r:id="rId27" xr:uid="{5703FE63-67D6-2A42-8863-2641493567D2}"/>
+    <hyperlink ref="D27" r:id="rId28" xr:uid="{450FD685-BCD3-DB4D-AF94-AE9997850DC8}"/>
+    <hyperlink ref="D28" r:id="rId29" xr:uid="{625D852E-45E1-9A44-A53E-C7797A8DEDCF}"/>
+    <hyperlink ref="D29" r:id="rId30" xr:uid="{CF41F5F8-462D-8B49-977F-6A6C535AAB34}"/>
+    <hyperlink ref="D30" r:id="rId31" xr:uid="{230F6A81-AAFB-B041-8CFF-0A28E8FA81F4}"/>
+    <hyperlink ref="D31" r:id="rId32" xr:uid="{AF19FE73-5D02-6542-B48C-7735B218346C}"/>
+    <hyperlink ref="D32" r:id="rId33" xr:uid="{7253B686-0DB5-C942-A9D7-F1B6CE4A9223}"/>
+    <hyperlink ref="D34" r:id="rId34" xr:uid="{18EAA52F-F37F-A648-B019-E9113CB6C960}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit on 2022-10-05 at 12:35:26
</commit_message>
<xml_diff>
--- a/submissions/pending.xlsx
+++ b/submissions/pending.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/distasl/Documents/WD/profDocs/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DA7439-0959-AE4B-9D89-64554F8905EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539821EE-BDDE-B649-B678-A69AE89B6CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{9CE22EEB-E98C-5749-B029-6028B6AD91A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="pending" localSheetId="0">Sheet1!$A$1:$E$35</definedName>
+    <definedName name="pending" localSheetId="0">Sheet1!$A$1:$E$32</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="97">
   <si>
     <t>Institute of Science and Technology Austria (ISTA)</t>
   </si>
@@ -63,6 +63,9 @@
     <t xml:space="preserve"> Assistant Professor (tenure-track) and Professor positions in all areas of sciences</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://www.nature.com/naturecareers/job/assistant-professor-tenuretrack-and-professor-positions-in-all-areas-of-sciences-institute-of-science-and-technology-austria-ista-762911</t>
+  </si>
+  <si>
     <t>King Fahd University of Petroleum &amp; Minerals</t>
   </si>
   <si>
@@ -72,6 +75,9 @@
     <t xml:space="preserve"> Assistant / Associate / Full Professor - Material Science and Engineering</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://jobs.kfupm.edu.sa/postings/1813</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -84,6 +90,9 @@
     <t xml:space="preserve"> Postdoc in network-inspired models of heterogeneous materials</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://www.nature.com/naturecareers/job/postdoc-in-networkinspired-models-of-heterogeneous-materials-aarhus-university-au-763330</t>
+  </si>
+  <si>
     <t>Syracuse University</t>
   </si>
   <si>
@@ -93,6 +102,9 @@
     <t xml:space="preserve"> Assistant Professor- Solid Mechanics</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://www.sujobopps.com/postings/94961</t>
+  </si>
+  <si>
     <t>Ghent University</t>
   </si>
   <si>
@@ -102,13 +114,7 @@
     <t xml:space="preserve"> Postdoc vacancy on computational mechanics of thick adhesive joints in large wind turbine blades</t>
   </si>
   <si>
-    <t>Technology Innovation Institute</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> UAE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Senior Researcher</t>
+    <t xml:space="preserve"> https://composites.ugent.be/PhD_job_vacancies_PhD_job_positions_composites.html</t>
   </si>
   <si>
     <t>University of Southern Denmark</t>
@@ -117,24 +123,36 @@
     <t xml:space="preserve"> Postdoc Position in Soft Robotic Locomotion Control and Learning</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://www.sdu.dk/en/service/ledige_stillinger/1195449</t>
+  </si>
+  <si>
     <t>Georgia Tech</t>
   </si>
   <si>
     <t xml:space="preserve"> Multi Rank Tenured/Tenure-Track Faculty Positions</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://careers.hprod.onehcm.usg.edu/psc/careers/CAREERS/HRMS/c/HRS_HRAM_FL.HRS_CG_SEARCH_FL.GBL?Page=HRS_APP_SCHJOB_FL&amp;Action=U</t>
+  </si>
+  <si>
     <t>Colorado School of Mines</t>
   </si>
   <si>
     <t xml:space="preserve"> Assistant Professor Mechanical Engineering Biomechanics</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://jobs.mines.edu/cw/en-us/job/495861/assistant-professor-mechanical-engineering-biomechanics</t>
+  </si>
+  <si>
     <t>UC San Diego</t>
   </si>
   <si>
     <t xml:space="preserve"> Assistant Professor in Aerospace Engineering</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://apol-recruit.ucsd.edu/JPF03339</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Assistant Teaching Professor (LPSOE) in Aerospace Engineering</t>
   </si>
   <si>
@@ -144,6 +162,9 @@
     <t xml:space="preserve"> Assistant or Associate Professor of Mechanical Engineering - Biomechanics</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://careers.purdue.edu/job/West-Lafayette-Assistant-or-Associate-Professor-of-Mechanical-Engineering-Biomechanics-IN-47906/932366300/</t>
+  </si>
+  <si>
     <t>University of Exeter</t>
   </si>
   <si>
@@ -153,37 +174,49 @@
     <t xml:space="preserve"> Lectureship with initial Research Fellowship in Materials Modelling and Simulation</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://jobs.exeter.ac.uk/hrpr_webrecruitment/wrd/run/ETREC107GF.open?VACANCY_ID=448681b4fm&amp;WVID=3817591jNg&amp;LANG=USA</t>
+  </si>
+  <si>
     <t>University of Nottingham</t>
   </si>
   <si>
     <t xml:space="preserve"> Nottingham Research Fellowships 2023</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://www.nottingham.ac.uk/jobs/currentvacancies/ref/NARF2023</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Assistant or Associate Professor in Solid Mechanics</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://www.sdu.dk/en/service/ledige_stillinger/1196606</t>
+  </si>
+  <si>
     <t xml:space="preserve"> IE</t>
   </si>
   <si>
     <t xml:space="preserve"> R&amp;D Engineer</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3124936927/?refId=943fb5ac-7d12-48fa-82c9-728b874e7b54&amp;trackingId=ncNGSaq3TFuRcNdtLWYfjA%3D%3D&amp;trk=flagship3_job_home_savedjobs</t>
+  </si>
+  <si>
     <t>Raytheon UK</t>
   </si>
   <si>
     <t xml:space="preserve"> Senior Mechanical Engineer</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3249299200/?refId=943fb5ac-7d12-48fa-82c9-728b874e7b54&amp;trackingId=V14blwBhRleNexF35IjHMg%3D%3D&amp;trk=flagship3_job_home_savedjobs</t>
+  </si>
+  <si>
     <t>Hays</t>
   </si>
   <si>
     <t xml:space="preserve"> Senior Mechanical Design Engineer</t>
   </si>
   <si>
-    <t>Floating Power Plant</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Research &amp; Development Naval Architect/Structural Engineer</t>
+    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3252949620/?refId=943fb5ac-7d12-48fa-82c9-728b874e7b54&amp;trackingId=iskLuf5pTmiMMUqzNQDOjQ%3D%3D&amp;trk=flagship3_job_home_savedjobs</t>
   </si>
   <si>
     <t>ServiceNow</t>
@@ -192,6 +225,9 @@
     <t xml:space="preserve"> EMEA Learning Manager</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3225612167/?alternateChannel=search&amp;refId=lJVuGicyUSnYYZkbYO6qzQ%3D%3D&amp;trackingId=0i56ToJcMXot%2FAJETWTlBQ%3D%3D&amp;trk=d_flagship3_search_srp_jobs</t>
+  </si>
+  <si>
     <t>Wikimedia Foundation</t>
   </si>
   <si>
@@ -201,6 +237,9 @@
     <t xml:space="preserve"> Technical Community Program Manager</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://boards.greenhouse.io/wikimedia/jobs/4496668</t>
+  </si>
+  <si>
     <t>RavenPack</t>
   </si>
   <si>
@@ -210,7 +249,7 @@
     <t xml:space="preserve"> Quantitative Researcher</t>
   </si>
   <si>
-    <t>NKT Photonics</t>
+    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3256966142/?alternateChannel=search&amp;refId=dAsMlpfljPkYMRsHnYIdcQ%3D%3D&amp;trackingId=0glUOyL4W8jbKnes5%2BtPpQ%3D%3D</t>
   </si>
   <si>
     <t>Mason Alexander</t>
@@ -219,52 +258,91 @@
     <t xml:space="preserve"> R&amp;D Technical Lead</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3278517624/?lgTemp=jobs_jymbii_digest&amp;eBP=NotAvailableFromMidTier&amp;lgCta=eml-jymbii-organic-job-card&amp;recommendedFlavor=HIDDEN_GEM&amp;refId=2CypfbVUooL1DKQxBBqnlg%3D%3D&amp;trackingId=2CypfbVUooL1DKQxBBqnlg%3D%3D&amp;midToken=AQGW6lN0ZhE6Zw&amp;midSig=1qW8sQGH0J7qs1&amp;trk=eml-jobs_jymbii_digest-jymbii-33-job_card_mercado&amp;trkEmail=eml-jobs_jymbii_digest-jymbii-33-job_card_mercado-null-242drh%7El8beweas%7Euf-null-jobs%7Eview</t>
+  </si>
+  <si>
     <t>UNICEF</t>
   </si>
   <si>
     <t xml:space="preserve"> Innovation Manager (WASH)</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3276000844/?lgTemp=jobs_jymbii_digest&amp;eBP=NotAvailableFromMidTier&amp;lgCta=eml-jymbii-organic-job-card&amp;recommendedFlavor=SCHOOL_RECRUIT&amp;refId=yGQcs9ybSngEdWVlEW7v3Q%3D%3D&amp;trackingId=yGQcs9ybSngEdWVlEW7v3Q%3D%3D&amp;midToken=AQGW6lN0ZhE6Zw&amp;midSig=0KvbZl5i5Aaas1&amp;trk=eml-jobs_jymbii_digest-jymbii-27-job_card_mercado&amp;trkEmail=eml-jobs_jymbii_digest-jymbii-27-job_card_mercado-null-242drh%7El8e9fvwr%7Exe-null-jobs%7Eview</t>
+  </si>
+  <si>
     <t>Fiberline Composites</t>
   </si>
   <si>
     <t xml:space="preserve"> Project Manager</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://www.innomate.com/InnomatePublicPagesMedarb/JobNotice.aspx?CompanyId=fiberline&amp;JobNoticeId=122</t>
+  </si>
+  <si>
     <t>Hollister</t>
   </si>
   <si>
     <t xml:space="preserve"> Senior R&amp;D Engineer</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3264064488/?refId=V%2FHpkFDpy62s7woTWC5YmQ%3D%3D&amp;trackingId=V%2FHpkFDpy62s7woTWC5YmQ%3D%3D&amp;midToken=AQGW6lN0ZhE6Zw&amp;midSig=0FiJf_T0kfjas1&amp;trk=eml-email_jobs_viewed_job_reminder_01-similar_jobs-64-similar%7Ejob%7Etitle%7Emercado&amp;trkEmail=eml-email_jobs_viewed_job_reminder_01-similar_jobs-64-similar%7Ejob%7Etitle%7Emercado-null-242drh%7El8nbn0pw%7E30-null-jobs%7Eview</t>
+  </si>
+  <si>
     <t>Real Staffing</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/3270262889/?refId=NXgPyne2BuIGhBW0wEsRbQ%3D%3D&amp;trackingId=NXgPyne2BuIGhBW0wEsRbQ%3D%3D&amp;midToken=AQGW6lN0ZhE6Zw&amp;midSig=0FiJf_T0kfjas1&amp;trk=eml-email_jobs_viewed_job_reminder_01-similar_jobs-60-similar%7Ejob%7Etitle%7Emercado&amp;trkEmail=eml-email_jobs_viewed_job_reminder_01-similar_jobs-60-similar%7Ejob%7Etitle%7Emercado-null-242drh%7El8nbn0pw%7E30-null-jobs%7Eview</t>
+  </si>
+  <si>
     <t>Julia Computing</t>
   </si>
   <si>
     <t xml:space="preserve"> Application Developer</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://jobs.juliacomputing.com/jobs/3NhVYuObq6cY/application-developer-remote</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Scientific Application Developer</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://jobs.juliacomputing.com/jobs/Ievy9W70_BjO/scientific-application-developer-remote</t>
+  </si>
+  <si>
     <t>Pale Blue DotÂ®Recruitment Limited</t>
   </si>
   <si>
     <t>Novo Nordisk</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://careers.novonordisk.com/job/HillerÃ¸d-Senior-R&amp;D-Engineer-Capi/854804001/</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Research Data Steward</t>
   </si>
   <si>
+    <t xml:space="preserve"> https://careers.novonordisk.com/job/MÃ¥lÃ¸v-Research-Data-Steward-Capi/850472801/</t>
+  </si>
+  <si>
     <t>Carpentries</t>
   </si>
   <si>
     <t xml:space="preserve"> Executive Council</t>
   </si>
   <si>
-    <t>view</t>
+    <t xml:space="preserve"> https://docs.google.com/forms/d/e/1FAIpQLSdMTiM5bjmF7Tq90BifM41eVWSlLL6tbD6eqKmtl8tAWkP23g/viewform</t>
+  </si>
+  <si>
+    <t>Copenaghen University</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Postdoc in computational fluid and solid mechanics</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://jobportal.ku.dk/videnskabelige-stillinger/?show=157437</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://apol-recruit.ucsd.edu/JPF03342</t>
   </si>
 </sst>
 </file>
@@ -309,13 +387,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
@@ -639,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526B7EBF-53BB-884F-AAF1-E7894D9216BC}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,8 +737,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>70</v>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="E1" s="2">
         <v>44858</v>
@@ -671,33 +746,33 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>70</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>70</v>
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="E3" s="2">
         <v>44849</v>
@@ -705,16 +780,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>70</v>
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="E4" s="2">
         <v>44849</v>
@@ -722,259 +797,268 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="2">
-        <v>44880</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>70</v>
+        <v>94</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="2">
+        <v>44866</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2">
+        <v>44849</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
+        <v>25</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2">
+        <v>44851</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
+        <v>28</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="2">
+        <v>44855</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>70</v>
+        <v>31</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="E10" s="2">
-        <v>44857</v>
+        <v>44848</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>70</v>
+        <v>33</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="E11" s="2">
-        <v>44865</v>
+        <v>44848</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>70</v>
+        <v>35</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="E12" s="2">
-        <v>44843</v>
+        <v>44896</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>70</v>
+        <v>39</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="2">
+        <v>44871</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>70</v>
+        <v>42</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="2">
+        <v>44840</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>70</v>
+      <c r="E15" s="2">
+        <v>44880</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" t="s">
-        <v>6</v>
+        <v>47</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>70</v>
+        <v>50</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="E17" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>70</v>
+        <v>53</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" t="s">
-        <v>6</v>
+        <v>56</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>70</v>
+        <v>60</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -982,283 +1066,193 @@
         <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>70</v>
+      <c r="D21" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="2">
-        <v>44851</v>
+      <c r="E22" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="5" t="s">
         <v>70</v>
       </c>
+      <c r="D23" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="E23" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="2">
-        <v>44871</v>
+        <v>76</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="2">
-        <v>44840</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>70</v>
+        <v>81</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="E27" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" t="s">
-        <v>6</v>
+        <v>83</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>70</v>
+        <v>76</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="E29" s="2">
-        <v>44849</v>
+        <v>44865</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>70</v>
+        <v>88</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="E30" s="2">
-        <v>44851</v>
+        <v>44843</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>70</v>
+        <v>91</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="E31" s="2">
-        <v>44855</v>
+        <v>44851</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E32" s="2">
-        <v>44848</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" s="2">
-        <v>44848</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E34" s="2">
-        <v>44896</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E35">
-    <sortCondition ref="B1:B35"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E32">
+    <sortCondition ref="B1:B32"/>
   </sortState>
-  <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1" xr:uid="{4B133E65-D92E-1543-AA75-04310E5BFC1E}"/>
-    <hyperlink ref="D11" r:id="rId2" xr:uid="{20B84960-8C50-A742-979E-A5D4829F3DC1}"/>
-    <hyperlink ref="D12" r:id="rId3" xr:uid="{D64DBDE8-111D-794C-9523-567730D88024}"/>
-    <hyperlink ref="D9" r:id="rId4" xr:uid="{99799B85-16A3-A14B-A8E7-450FC0E3092D}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{98BADD85-0200-FC4B-AED6-28EF3DFBAA0A}"/>
-    <hyperlink ref="D6" r:id="rId6" xr:uid="{32CD9F87-5983-694F-81E4-624893AC0C09}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{62232260-DB6F-9A40-9A29-0DE8F7884E68}"/>
-    <hyperlink ref="D33" r:id="rId8" xr:uid="{A88AFDAB-EB57-A44F-B93A-4A64DFE6CE6B}"/>
-    <hyperlink ref="D1" r:id="rId9" xr:uid="{5806C2F7-7A0A-1B42-975F-24FC659F7AF3}"/>
-    <hyperlink ref="D2" r:id="rId10" xr:uid="{7FDB8605-1B30-F741-B74B-95E2C37C703E}"/>
-    <hyperlink ref="D3" r:id="rId11" xr:uid="{E46C9387-595E-A146-A5C6-2F52A948F1B8}"/>
-    <hyperlink ref="D4" r:id="rId12" xr:uid="{29ABE021-E5BF-BA48-8FE8-FFBBF41B5B18}"/>
-    <hyperlink ref="D5" r:id="rId13" xr:uid="{7E7C2147-CD4A-914F-9E39-17834782CD24}"/>
-    <hyperlink ref="D13" r:id="rId14" xr:uid="{A1881E4E-16C6-A047-9D87-49FBF3BA885E}"/>
-    <hyperlink ref="D14" r:id="rId15" xr:uid="{58C4C5F6-D88E-6A41-8286-DFE5ABE5AFE4}"/>
-    <hyperlink ref="D15" r:id="rId16" xr:uid="{11361235-E0CA-5742-91A1-FC72BEFBFCD9}"/>
-    <hyperlink ref="D16" r:id="rId17" xr:uid="{1F055798-6460-5E4E-B1EE-F251CB0F6DBE}"/>
-    <hyperlink ref="D17" r:id="rId18" xr:uid="{7C62CE5E-6D3E-174A-B7A6-66AE57580976}"/>
-    <hyperlink ref="D18" r:id="rId19" xr:uid="{A1301579-4623-604F-87B9-862DAC929BAD}"/>
-    <hyperlink ref="D19" r:id="rId20" xr:uid="{3124D040-ACDD-0747-8E1B-5B8DCD5F3F5F}"/>
-    <hyperlink ref="D20" r:id="rId21" xr:uid="{47AF3DA8-DF4A-4D47-96DA-0FF7BA634481}"/>
-    <hyperlink ref="D21" r:id="rId22" xr:uid="{4EC961BF-5212-1547-ABC6-F12C92CDF8DA}"/>
-    <hyperlink ref="D22" r:id="rId23" xr:uid="{7984A528-6DCD-9340-85FB-95BC4BF499E7}"/>
-    <hyperlink ref="D23" r:id="rId24" xr:uid="{67B3F2F8-C645-DF47-B54D-F50486927AB7}"/>
-    <hyperlink ref="D24" r:id="rId25" xr:uid="{857C5379-06A9-614F-9C37-5F7E3B71FC07}"/>
-    <hyperlink ref="D25" r:id="rId26" xr:uid="{D46B45D8-1EEB-E84A-9A6D-8419E5353BC9}"/>
-    <hyperlink ref="D26" r:id="rId27" xr:uid="{5703FE63-67D6-2A42-8863-2641493567D2}"/>
-    <hyperlink ref="D27" r:id="rId28" xr:uid="{450FD685-BCD3-DB4D-AF94-AE9997850DC8}"/>
-    <hyperlink ref="D28" r:id="rId29" xr:uid="{625D852E-45E1-9A44-A53E-C7797A8DEDCF}"/>
-    <hyperlink ref="D29" r:id="rId30" xr:uid="{CF41F5F8-462D-8B49-977F-6A6C535AAB34}"/>
-    <hyperlink ref="D30" r:id="rId31" xr:uid="{230F6A81-AAFB-B041-8CFF-0A28E8FA81F4}"/>
-    <hyperlink ref="D31" r:id="rId32" xr:uid="{AF19FE73-5D02-6542-B48C-7735B218346C}"/>
-    <hyperlink ref="D32" r:id="rId33" xr:uid="{7253B686-0DB5-C942-A9D7-F1B6CE4A9223}"/>
-    <hyperlink ref="D34" r:id="rId34" xr:uid="{18EAA52F-F37F-A648-B019-E9113CB6C960}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>